<commit_message>
anchor thumbnail base code#2
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="140">
   <si>
     <t>Want to do</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -584,6 +584,10 @@
   </si>
   <si>
     <t>신규 시나리오</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터를 log 스케일로 바꿔보는거 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1088,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1616,7 +1620,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
-        <v>43082</v>
+        <v>43083</v>
       </c>
       <c r="B56" t="s">
         <v>126</v>
@@ -1696,22 +1700,25 @@
         <v>110</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C65" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C66" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C67" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D67" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <v>43086</v>
       </c>
@@ -1722,7 +1729,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
         <v>43086</v>
       </c>
@@ -1733,32 +1740,32 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C70" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C71" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>119</v>
       </c>

</xml_diff>

<commit_message>
add node detail parameters view
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Lectures\17-2 InfoVis\Infovis term project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Lectures\17-2 InfoVis\ReVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10095" yWindow="0" windowWidth="14835" windowHeight="10335" activeTab="1"/>
+    <workbookView xWindow="11235" yWindow="0" windowWidth="12390" windowHeight="10335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="145">
   <si>
     <t>Want to do</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -552,10 +551,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>detail 구현</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>reuse - same data</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -589,6 +584,30 @@
   </si>
   <si>
     <t>데이터를 log 스케일로 바꿔보는거 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>detail tree 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이상한 링크 삭제, 라인 차트 오류 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이은</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구현 후 결정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default 화면 수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -653,7 +672,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -672,8 +691,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1093,13 +1118,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.75" customWidth="1"/>
+    <col min="1" max="1" width="11.75" style="6" customWidth="1"/>
     <col min="2" max="2" width="13.25" customWidth="1"/>
     <col min="3" max="3" width="37.125" customWidth="1"/>
     <col min="5" max="5" width="47.125" customWidth="1"/>
@@ -1107,7 +1132,7 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>88</v>
       </c>
       <c r="B4" t="s">
@@ -1124,7 +1149,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>89</v>
       </c>
       <c r="B5" t="s">
@@ -1144,7 +1169,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>89</v>
       </c>
       <c r="B6" t="s">
@@ -1161,7 +1186,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>88</v>
       </c>
       <c r="B7" t="s">
@@ -1178,7 +1203,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="6" t="s">
         <v>88</v>
       </c>
       <c r="B8" t="s">
@@ -1198,7 +1223,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="6" t="s">
         <v>88</v>
       </c>
       <c r="B9" t="s">
@@ -1215,7 +1240,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="6" t="s">
         <v>88</v>
       </c>
       <c r="B10" t="s">
@@ -1232,7 +1257,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="6" t="s">
         <v>88</v>
       </c>
       <c r="B11" t="s">
@@ -1249,7 +1274,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="6" t="s">
         <v>88</v>
       </c>
       <c r="B12" t="s">
@@ -1266,7 +1291,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="6" t="s">
         <v>88</v>
       </c>
       <c r="B13" t="s">
@@ -1297,6 +1322,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
       <c r="C15" s="3" t="s">
         <v>30</v>
       </c>
@@ -1308,7 +1334,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -1322,7 +1348,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="6" t="s">
         <v>88</v>
       </c>
       <c r="B17" t="s">
@@ -1339,7 +1365,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -1353,7 +1379,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1367,6 +1393,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
       <c r="C20" s="3" t="s">
         <v>30</v>
       </c>
@@ -1378,6 +1405,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
       <c r="C21" s="3" t="s">
         <v>30</v>
       </c>
@@ -1389,7 +1417,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1403,6 +1431,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
       <c r="C23" s="3" t="s">
         <v>30</v>
       </c>
@@ -1609,8 +1638,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>133</v>
+      <c r="A55" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="B55" t="s">
         <v>126</v>
@@ -1620,8 +1649,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="6">
-        <v>43083</v>
+      <c r="A56" s="8" t="s">
+        <v>139</v>
       </c>
       <c r="B56" t="s">
         <v>126</v>
@@ -1631,18 +1660,18 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="6">
+      <c r="A57" s="8">
         <v>43083</v>
       </c>
       <c r="B57" t="s">
         <v>126</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+      <c r="A58" s="6" t="s">
         <v>117</v>
       </c>
       <c r="B58" t="s">
@@ -1653,8 +1682,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="6">
-        <v>43083</v>
+      <c r="A59" s="8">
+        <v>43085</v>
       </c>
       <c r="B59" t="s">
         <v>127</v>
@@ -1664,8 +1693,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="6">
-        <v>43082</v>
+      <c r="A60" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="B60" t="s">
         <v>127</v>
@@ -1675,80 +1704,109 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="6">
-        <v>43084</v>
+      <c r="A61" s="8">
+        <v>43083</v>
       </c>
       <c r="B61" t="s">
         <v>127</v>
       </c>
       <c r="C61" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="8"/>
+      <c r="B62" t="s">
+        <v>142</v>
+      </c>
+      <c r="C62" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="8">
+        <v>43085</v>
+      </c>
+      <c r="C63" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="6"/>
-      <c r="C62" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C63" t="s">
-        <v>129</v>
-      </c>
-    </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="8">
+        <v>43075</v>
+      </c>
       <c r="C64" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="8">
+        <v>43075</v>
+      </c>
       <c r="C65" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="8">
+        <v>43085</v>
+      </c>
       <c r="C66" t="s">
-        <v>124</v>
+        <v>136</v>
+      </c>
+      <c r="D66" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="8"/>
       <c r="C67" t="s">
-        <v>137</v>
-      </c>
-      <c r="D67" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="6">
+      <c r="A68" s="8">
         <v>43086</v>
       </c>
       <c r="B68" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C68" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="6">
+      <c r="A69" s="8">
         <v>43086</v>
       </c>
       <c r="B69" t="s">
         <v>126</v>
       </c>
       <c r="C69" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="C70" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C71" t="s">
-        <v>138</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C73" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add filtertop function remove unused console log
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="145">
   <si>
     <t>Want to do</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -499,10 +499,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>O</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>reasoning process =&gt; exploration path?  =&gt; 그냥 유추해볼 수 있다. 정도로 해도 될 듯</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -555,14 +551,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>reuse - new data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>O</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>report 작성</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -587,10 +575,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>O</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>detail tree 구현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -608,6 +592,22 @@
   </si>
   <si>
     <t>default 화면 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reuse - new data(bmi 데이터)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이은</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영택</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -644,7 +644,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -654,6 +654,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -672,7 +678,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -699,6 +705,12 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1119,7 +1131,7 @@
   <dimension ref="A4:F83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1619,7 +1631,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1639,65 +1651,65 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="B55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C55" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="8" t="s">
-        <v>139</v>
+      <c r="A56" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="B56" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="8">
-        <v>43083</v>
+      <c r="A57" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="B57" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="B58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C58" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="8">
+    <row r="59" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="9">
         <v>43085</v>
       </c>
-      <c r="B59" t="s">
-        <v>127</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="B59" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C59" s="10" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="B60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>116</v>
@@ -1708,43 +1720,51 @@
         <v>43083</v>
       </c>
       <c r="B61" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C61" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="8"/>
+      <c r="A62" s="6" t="s">
+        <v>141</v>
+      </c>
       <c r="B62" t="s">
+        <v>138</v>
+      </c>
+      <c r="C62" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="9">
+        <v>43085</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C63" s="10" t="s">
         <v>142</v>
-      </c>
-      <c r="C62" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="8">
-        <v>43085</v>
-      </c>
-      <c r="C63" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="8">
-        <v>43075</v>
+        <v>43085</v>
       </c>
       <c r="C64" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="9">
+        <v>43084</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C65" s="10" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="8">
-        <v>43075</v>
-      </c>
-      <c r="C65" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1752,43 +1772,43 @@
         <v>43085</v>
       </c>
       <c r="C66" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D66" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="8"/>
       <c r="C67" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="8">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="9">
         <v>43086</v>
       </c>
-      <c r="B68" t="s">
-        <v>135</v>
-      </c>
-      <c r="C68" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="8">
+      <c r="B68" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="9">
         <v>43086</v>
       </c>
-      <c r="B69" t="s">
-        <v>126</v>
-      </c>
-      <c r="C69" t="s">
-        <v>133</v>
+      <c r="B69" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C70" t="s">
         <v>109</v>
@@ -1796,12 +1816,12 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C71" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1811,7 +1831,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -1826,17 +1846,17 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>